<commit_message>
20230114 Pyspark GroupBy And Aggregate datafile
</commit_message>
<xml_diff>
--- a/Notes/03 Pyspark with Python/test1.xlsx
+++ b/Notes/03 Pyspark with Python/test1.xlsx
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="A1:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>